<commit_message>
Added USB slow plug CAP, corrected BOM errors updated documentation and layout
</commit_message>
<xml_diff>
--- a/SJ2096POE_R0M0E0/Docs/Assembly Outputs/BOM/BOM-SJ2096POE(Production).xlsx
+++ b/SJ2096POE_R0M0E0/Docs/Assembly Outputs/BOM/BOM-SJ2096POE(Production).xlsx
@@ -1,42 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal\luxonis\depthai-hardware2\MB2096POE_R2M1E2\PCB\KingTop_Output_Files\Assembly Outputs\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{660F9F05-F84A-4F07-8B05-956CEC90AD8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{BCD5F692-9047-4BA3-A0A3-E7BD7D3804D0}"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="27795" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-SJ2096POE(Production)" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'BOM-SJ2096POE(Production)'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="386">
   <si>
     <t>Comment</t>
   </si>
@@ -209,7 +192,7 @@
     <t>1uF 0402</t>
   </si>
   <si>
-    <t>C11, C46, C47</t>
+    <t>C11, C46, C47, C51</t>
   </si>
   <si>
     <t>CAP CER 1UF 25V X5R 0402 10%</t>
@@ -416,22 +399,19 @@
     <t>SML-D12U8WT86</t>
   </si>
   <si>
-    <t>CD-HD01, BW2098_A Receptacle, BW2098_B Receptacle, CX80B1-24P USB-C VERT</t>
-  </si>
-  <si>
-    <t>D8, D9, J2, J3, J10</t>
-  </si>
-  <si>
-    <t>CD-HD0x Series Schottky Bridge Rectifier Diode 100V 4-Pin Surface Mount T/R, CONN RCPT 100POS 0.4MM SMD GOLD BW2098_A Receptacle, CONN RCPT 100POS 0.4MM SMD GOLD BW2098_B Receptacle, USB - C USB 3.0 (USB 3.1 Gen 1 Superspeed) Male Receptacle Connector 24 Position</t>
-  </si>
-  <si>
-    <t>[NoParam], Hirose</t>
-  </si>
-  <si>
-    <t>CD-H01, DF40HC-3.0-100DS-0.4V_minpad, CX80B1-24P</t>
-  </si>
-  <si>
-    <t>CD-HD01, DF40HC(3.0)-100DS-0.4V_BW2098_A, DF40HC(3.0)-100DS-0.4V_BW2098_B, CX80B1-24P</t>
+    <t>CD-HD01</t>
+  </si>
+  <si>
+    <t>D8, D9</t>
+  </si>
+  <si>
+    <t>CD-HD0x Series Schottky Bridge Rectifier Diode 100V 4-Pin Surface Mount T/R</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>CD-H01</t>
   </si>
   <si>
     <t>GREEN 0603</t>
@@ -506,6 +486,27 @@
     <t>TRJG0926HENL</t>
   </si>
   <si>
+    <t>BW2098_A Receptacle, BW2098_B Receptacle</t>
+  </si>
+  <si>
+    <t>J2, J3</t>
+  </si>
+  <si>
+    <t>CONN RCPT 100POS 0.4MM SMD GOLD BW2098_A Receptacle, CONN RCPT 100POS 0.4MM SMD GOLD BW2098_B Receptacle</t>
+  </si>
+  <si>
+    <t>Hirose</t>
+  </si>
+  <si>
+    <t>DF40HC(3.0)-100DS-0.4V(58)</t>
+  </si>
+  <si>
+    <t>DF40HC-3.0-100DS-0.4V_minpad</t>
+  </si>
+  <si>
+    <t>DF40HC(3.0)-100DS-0.4V_BW2098_A, DF40HC(3.0)-100DS-0.4V_BW2098_B</t>
+  </si>
+  <si>
     <t>SFV10R-2STE1HLF Top Contact</t>
   </si>
   <si>
@@ -564,6 +565,18 @@
   </si>
   <si>
     <t>A12N02A-201_Connector_(1.6mm_brd)</t>
+  </si>
+  <si>
+    <t>CX80B1-24P USB-C VERT</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB - C USB 3.0 (USB 3.1 Gen 1 Superspeed) Male Receptacle Connector 24 Position</t>
+  </si>
+  <si>
+    <t>CX80B1-24P</t>
   </si>
   <si>
     <t>1uH 2.9A</t>
@@ -1169,13 +1182,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1220,7 +1234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1232,6 +1246,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,9 +1258,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1260,44 +1274,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1325,31 +1339,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1377,23 +1374,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1405,151 +1385,175 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56CF9E2-5F20-4562-9A3C-36199F73F0B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1860,7 +1864,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>57</v>
@@ -2319,12 +2323,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B27" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>127</v>
@@ -2335,569 +2339,571 @@
       <c r="E27" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>130</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>111</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>113</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29" s="4">
         <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="F29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="H30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" s="4">
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="G31" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="4">
+        <v>2</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>160</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="4">
         <v>2</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="4">
-        <v>1</v>
-      </c>
       <c r="C35" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="G35" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>174</v>
       </c>
       <c r="H36" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B37" s="4">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="I37" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="G38" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>190</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B40" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>198</v>
+        <v>34</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B42" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E42" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B43" s="4">
+      <c r="F44" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" s="4">
         <v>3</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="C45" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B44" s="4">
+      <c r="F45" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="4">
         <v>10</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F46" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="H46" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>223</v>
       </c>
@@ -2911,367 +2917,367 @@
         <v>225</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G47" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="I47" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B48" s="4">
+      <c r="H48" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B50" s="4">
         <v>27</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
       <c r="C50" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B56" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B58" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B59" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G59" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H59" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="H59" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="I59" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3279,7 +3285,7 @@
         <v>279</v>
       </c>
       <c r="B60" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>280</v>
@@ -3288,13 +3294,13 @@
         <v>281</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>282</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>212</v>
+        <v>283</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>282</v>
@@ -3305,205 +3311,205 @@
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B61" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>212</v>
+        <v>288</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B63" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B64" s="4">
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>278</v>
+        <v>222</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B65" s="4">
         <v>2</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>212</v>
+        <v>305</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B66" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>212</v>
+        <v>288</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B67" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>311</v>
+        <v>226</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G67" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="H67" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="I67" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3511,7 +3517,7 @@
         <v>314</v>
       </c>
       <c r="B68" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>315</v>
@@ -3520,135 +3526,135 @@
         <v>316</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>314</v>
+        <v>222</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B69" s="4">
         <v>1</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B70" s="4">
         <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D70" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="G70" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B71" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C71" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="G71" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B72" s="4">
         <v>1</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D72" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="G72" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3656,7 +3662,7 @@
         <v>336</v>
       </c>
       <c r="B73" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>337</v>
@@ -3665,7 +3671,7 @@
         <v>338</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>339</v>
@@ -3694,256 +3700,356 @@
         <v>342</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>340</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B75" s="4">
         <v>1</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B76" s="4">
         <v>1</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>139</v>
+        <v>330</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>350</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B77" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D77" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E77" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>354</v>
-      </c>
       <c r="H77" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B78" s="4">
         <v>1</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D78" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="G78" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>355</v>
-      </c>
       <c r="H78" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B79" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B80" s="4">
         <v>1</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D80" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="G80" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>366</v>
-      </c>
       <c r="H80" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B81" s="4">
         <v>1</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D81" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G81" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="E81" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>370</v>
-      </c>
       <c r="H81" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B82" s="4">
         <v>1</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>374</v>
+        <v>138</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B83" s="4">
+        <v>1</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B84" s="4">
+        <v>1</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="20" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="20" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>